<commit_message>
Added new changes and create surrogate folder
</commit_message>
<xml_diff>
--- a/optimiser/input/__index__.xlsx
+++ b/optimiser/input/__index__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\src\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954D2B3E-6637-4245-BC6B-733AE1766971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7231FD-48FA-4511-951C-585D261B0AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="19080" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="19080" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
   <si>
     <t>test</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>material</t>
+  </si>
+  <si>
+    <t>G39</t>
+  </si>
+  <si>
+    <t>G52</t>
+  </si>
+  <si>
+    <t>G30</t>
+  </si>
+  <si>
+    <t>G18</t>
   </si>
 </sst>
 </file>
@@ -226,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,12 +292,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +816,7 @@
       <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="14">
         <v>617</v>
       </c>
       <c r="C11" s="14">
@@ -833,7 +839,7 @@
       <c r="A12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="14">
         <v>617</v>
       </c>
       <c r="C12" s="14">
@@ -876,94 +882,186 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="12">
+        <v>617</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="12">
+        <v>11</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="14">
+        <v>617</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="14">
+        <v>12</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="14">
+        <v>617</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="14">
+        <v>13</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="16">
+        <v>617</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1000</v>
+      </c>
+      <c r="D17" s="16">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="20">
-        <v>617</v>
-      </c>
-      <c r="C14" s="18">
-        <v>800</v>
-      </c>
-      <c r="D14" s="18">
+      <c r="B18" s="18">
+        <v>617</v>
+      </c>
+      <c r="C18" s="18">
+        <v>800</v>
+      </c>
+      <c r="D18" s="18">
         <v>0</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="F18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="20">
-        <v>617</v>
-      </c>
-      <c r="C15" s="18">
-        <v>800</v>
-      </c>
-      <c r="D15" s="18">
+      <c r="B19" s="18">
+        <v>617</v>
+      </c>
+      <c r="C19" s="18">
+        <v>800</v>
+      </c>
+      <c r="D19" s="18">
         <v>0</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="18" t="s">
+      <c r="F19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="20">
-        <v>617</v>
-      </c>
-      <c r="C16" s="18">
-        <v>800</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="B20" s="18">
+        <v>617</v>
+      </c>
+      <c r="C20" s="18">
+        <v>800</v>
+      </c>
+      <c r="D20" s="18">
         <v>0</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="18" t="s">
+      <c r="F20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="20">
-        <v>617</v>
-      </c>
-      <c r="C17" s="18">
-        <v>800</v>
-      </c>
-      <c r="D17" s="18">
+      <c r="B21" s="18">
+        <v>617</v>
+      </c>
+      <c r="C21" s="18">
+        <v>800</v>
+      </c>
+      <c r="D21" s="18">
         <v>0</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="18" t="s">
+      <c r="F21" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="18" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added quadratic interpolation for critical damage for evpwd
</commit_message>
<xml_diff>
--- a/optimiser/input/__index__.xlsx
+++ b/optimiser/input/__index__.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7231FD-48FA-4511-951C-585D261B0AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC21167-2DAC-4FB2-B2FF-078DC8F7CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="4155" windowWidth="19080" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4335" windowWidth="19080" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t>test</t>
   </si>
@@ -118,6 +118,30 @@
   </si>
   <si>
     <t>G18</t>
+  </si>
+  <si>
+    <t>G42</t>
+  </si>
+  <si>
+    <t>G40</t>
+  </si>
+  <si>
+    <t>G21</t>
+  </si>
+  <si>
+    <t>G19</t>
+  </si>
+  <si>
+    <t>G63</t>
+  </si>
+  <si>
+    <t>G48</t>
+  </si>
+  <si>
+    <t>G51</t>
+  </si>
+  <si>
+    <t>G38</t>
   </si>
 </sst>
 </file>
@@ -133,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,43 +170,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -238,8 +232,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -255,45 +261,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,156 +554,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00724CD-5AEE-4E14-A7E6-D7422F85292E}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>617</v>
+      </c>
+      <c r="C2" s="2">
+        <v>800</v>
+      </c>
+      <c r="D2" s="2">
+        <v>80</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
-        <v>617</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B3" s="12">
+        <v>617</v>
+      </c>
+      <c r="C3" s="12">
         <v>800</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="12">
         <v>60</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="E3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12">
+        <v>617</v>
+      </c>
+      <c r="C4" s="12">
+        <v>800</v>
+      </c>
+      <c r="D4" s="12">
+        <v>65</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="8">
+        <v>617</v>
+      </c>
+      <c r="C5" s="8">
+        <v>800</v>
+      </c>
+      <c r="D5" s="8">
+        <v>70</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6">
-        <v>617</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B6" s="10">
+        <v>617</v>
+      </c>
+      <c r="C6" s="10">
         <v>800</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D6" s="10">
         <v>60</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4">
-        <v>617</v>
-      </c>
-      <c r="C4" s="4">
-        <v>800</v>
-      </c>
-      <c r="D4" s="4">
-        <v>65</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="6">
-        <v>617</v>
-      </c>
-      <c r="C5" s="6">
-        <v>800</v>
-      </c>
-      <c r="D5" s="6">
-        <v>65</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8">
-        <v>617</v>
-      </c>
-      <c r="C6" s="8">
-        <v>800</v>
-      </c>
-      <c r="D6" s="8">
-        <v>70</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="10">
         <v>617</v>
@@ -731,65 +712,65 @@
         <v>800</v>
       </c>
       <c r="D7" s="10">
+        <v>65</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10">
+        <v>617</v>
+      </c>
+      <c r="C8" s="10">
+        <v>800</v>
+      </c>
+      <c r="D8" s="10">
         <v>70</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4">
-        <v>617</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="E8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4">
+        <v>617</v>
+      </c>
+      <c r="C9" s="4">
         <v>800</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>80</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="6">
-        <v>617</v>
-      </c>
-      <c r="C9" s="6">
-        <v>800</v>
-      </c>
-      <c r="D9" s="6">
-        <v>80</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
@@ -812,256 +793,440 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="14">
-        <v>617</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="B11" s="12">
+        <v>617</v>
+      </c>
+      <c r="C11" s="12">
         <v>900</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>28</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="E11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14">
-        <v>617</v>
-      </c>
-      <c r="C12" s="14">
+      <c r="B12" s="12">
+        <v>617</v>
+      </c>
+      <c r="C12" s="12">
         <v>900</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>31</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="E12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="16">
-        <v>617</v>
-      </c>
-      <c r="C13" s="16">
+      <c r="B13" s="12">
+        <v>617</v>
+      </c>
+      <c r="C13" s="12">
         <v>900</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="12">
         <v>36</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6">
+        <v>617</v>
+      </c>
+      <c r="C14" s="6">
+        <v>900</v>
+      </c>
+      <c r="D14" s="6">
+        <v>26</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="10">
+        <v>617</v>
+      </c>
+      <c r="C15" s="10">
+        <v>900</v>
+      </c>
+      <c r="D15" s="10">
+        <v>28</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="10">
+        <v>617</v>
+      </c>
+      <c r="C16" s="10">
+        <v>900</v>
+      </c>
+      <c r="D16" s="10">
+        <v>31</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="10">
+        <v>617</v>
+      </c>
+      <c r="C17" s="10">
+        <v>900</v>
+      </c>
+      <c r="D17" s="10">
+        <v>36</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4">
+        <v>617</v>
+      </c>
+      <c r="C18" s="4">
+        <v>900</v>
+      </c>
+      <c r="D18" s="4">
+        <v>36</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="12">
-        <v>617</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="B19" s="12">
+        <v>617</v>
+      </c>
+      <c r="C19" s="12">
         <v>1000</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D19" s="12">
         <v>11</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="E19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="14">
-        <v>617</v>
-      </c>
-      <c r="C15" s="14">
+      <c r="B20" s="12">
+        <v>617</v>
+      </c>
+      <c r="C20" s="12">
         <v>1000</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D20" s="12">
         <v>12</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="E20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="14">
-        <v>617</v>
-      </c>
-      <c r="C16" s="14">
+      <c r="B21" s="12">
+        <v>617</v>
+      </c>
+      <c r="C21" s="12">
         <v>1000</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D21" s="12">
         <v>13</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="E21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="16">
-        <v>617</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="B22" s="12">
+        <v>617</v>
+      </c>
+      <c r="C22" s="12">
         <v>1000</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D22" s="12">
         <v>16</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="E22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="6">
+        <v>617</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="6">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="10">
+        <v>617</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1000</v>
+      </c>
+      <c r="D24" s="10">
+        <v>13</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4">
+        <v>617</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D25" s="4">
+        <v>16</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="18">
-        <v>617</v>
-      </c>
-      <c r="C18" s="18">
+      <c r="B26" s="10">
+        <v>617</v>
+      </c>
+      <c r="C26" s="10">
         <v>800</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D26" s="10">
         <v>0</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="18" t="s">
+      <c r="F26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="18">
-        <v>617</v>
-      </c>
-      <c r="C19" s="18">
+      <c r="B27" s="10">
+        <v>617</v>
+      </c>
+      <c r="C27" s="10">
         <v>800</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D27" s="10">
         <v>0</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="18" t="s">
+      <c r="F27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="18">
-        <v>617</v>
-      </c>
-      <c r="C20" s="18">
+      <c r="B28" s="10">
+        <v>617</v>
+      </c>
+      <c r="C28" s="10">
         <v>800</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D28" s="10">
         <v>0</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="18" t="s">
+      <c r="F28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="18">
-        <v>617</v>
-      </c>
-      <c r="C21" s="18">
+      <c r="B29" s="10">
+        <v>617</v>
+      </c>
+      <c r="C29" s="10">
         <v>800</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D29" s="10">
         <v>0</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E29" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="18" t="s">
+      <c r="F29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reduced MIN_DATA, and optimisation improvements
</commit_message>
<xml_diff>
--- a/optimiser/input/__index__.xlsx
+++ b/optimiser/input/__index__.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16E3FB6-4B63-42CC-90BC-CFDCADA5F2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF76222-6588-4076-B6EA-C765D4DE463F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="inl_1" sheetId="3" r:id="rId1"/>
-    <sheet name="inl_2" sheetId="14" r:id="rId2"/>
-    <sheet name="kaeri_aged" sheetId="10" r:id="rId3"/>
-    <sheet name="kaeri_base" sheetId="11" r:id="rId4"/>
-    <sheet name="kaeri_naged" sheetId="12" r:id="rId5"/>
+    <sheet name="params" sheetId="15" r:id="rId1"/>
+    <sheet name="inl_1" sheetId="3" r:id="rId2"/>
+    <sheet name="inl_2" sheetId="14" r:id="rId3"/>
+    <sheet name="kaeri_aged" sheetId="10" r:id="rId4"/>
+    <sheet name="kaeri_base" sheetId="11" r:id="rId5"/>
+    <sheet name="kaeri_naged" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="152">
   <si>
     <t>temp</t>
   </si>
@@ -452,6 +453,39 @@
   </si>
   <si>
     <t>large tertiary</t>
+  </si>
+  <si>
+    <t>evpcd</t>
+  </si>
+  <si>
+    <t>evp_s0</t>
+  </si>
+  <si>
+    <t>evp_R</t>
+  </si>
+  <si>
+    <t>evp_d</t>
+  </si>
+  <si>
+    <t>evp_n</t>
+  </si>
+  <si>
+    <t>evp_eta</t>
+  </si>
+  <si>
+    <t>cd_A</t>
+  </si>
+  <si>
+    <t>cd_xi</t>
+  </si>
+  <si>
+    <t>cd_phi</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>params</t>
   </si>
 </sst>
 </file>
@@ -566,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,6 +669,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,15 +785,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>59991</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>30224</xdr:rowOff>
+      <xdr:colOff>30683</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15570</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>274302</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>184122</xdr:rowOff>
+      <xdr:colOff>244994</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>169468</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -776,7 +816,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8881606" y="3268724"/>
+          <a:off x="8852298" y="3444570"/>
           <a:ext cx="2038715" cy="1487398"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1156,15 +1196,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>63572</xdr:rowOff>
+      <xdr:rowOff>82622</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1187,7 +1227,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8924925" y="5543550"/>
+          <a:off x="8896350" y="5562600"/>
           <a:ext cx="2628900" cy="1949522"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1506,11 +1546,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1902F50F-2185-47BD-872D-696190D94151}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="29">
+        <v>800</v>
+      </c>
+      <c r="C3" s="29">
+        <v>48.960209999999996</v>
+      </c>
+      <c r="D3" s="29">
+        <v>17.822620000000001</v>
+      </c>
+      <c r="E3" s="29">
+        <v>9.5687479999999994</v>
+      </c>
+      <c r="F3" s="29">
+        <v>2.0310410000000001</v>
+      </c>
+      <c r="G3" s="29">
+        <v>56309.59</v>
+      </c>
+      <c r="H3" s="29">
+        <v>1995.8009999999999</v>
+      </c>
+      <c r="I3" s="29">
+        <v>5.4386010000000002</v>
+      </c>
+      <c r="J3" s="29">
+        <v>6.7901199999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="29">
+        <v>900</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0.56735100000000005</v>
+      </c>
+      <c r="D4" s="29">
+        <v>24.645340000000001</v>
+      </c>
+      <c r="E4" s="29">
+        <v>34.15175</v>
+      </c>
+      <c r="F4" s="29">
+        <v>2.103748</v>
+      </c>
+      <c r="G4" s="29">
+        <v>31803.17</v>
+      </c>
+      <c r="H4" s="29">
+        <v>2679.5309999999999</v>
+      </c>
+      <c r="I4" s="29">
+        <v>4.1550710000000004</v>
+      </c>
+      <c r="J4" s="29">
+        <v>9.2708449999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="29">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="29">
+        <v>7.805677766819759</v>
+      </c>
+      <c r="D5" s="29">
+        <v>3.6500284236445503E-2</v>
+      </c>
+      <c r="E5" s="29">
+        <v>6.9933056799717779</v>
+      </c>
+      <c r="F5" s="29">
+        <v>2.1865293117519431</v>
+      </c>
+      <c r="G5" s="29">
+        <v>20539.05912569529</v>
+      </c>
+      <c r="H5" s="29">
+        <v>2388.9208062275929</v>
+      </c>
+      <c r="I5" s="29">
+        <v>3.5917325254613259</v>
+      </c>
+      <c r="J5" s="29">
+        <v>6.7517952580115246</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72057042-979B-4A98-BA2E-14DCB6564B56}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,12 +2511,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9578FDA3-F26E-4E35-80A8-9B064AEAD5AE}">
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,12 +3490,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539DB0F7-233D-4937-914F-C567FE238855}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3676,12 +3871,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69278EA8-6F9F-49D4-BBEE-C6F7D2601391}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V45" sqref="V45"/>
+    <sheetView topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5178,12 +5373,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F7E390-41A9-48B3-83EA-F302D713C1F5}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed up vs_czm and no_czm scripts
</commit_message>
<xml_diff>
--- a/optimiser/input/__index__.xlsx
+++ b/optimiser/input/__index__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE3EF4C-78C5-4F1D-AEE9-0827A07E8B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37E612E-5759-4135-A3B1-6F95B9947D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inl_1" sheetId="3" r:id="rId1"/>
@@ -2788,7 +2788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9578FDA3-F26E-4E35-80A8-9B064AEAD5AE}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3858,8 +3858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539DB0F7-233D-4937-914F-C567FE238855}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4274,8 +4274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69278EA8-6F9F-49D4-BBEE-C6F7D2601391}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5913,8 +5913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F7E390-41A9-48B3-83EA-F302D713C1F5}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected youngs modulus and poissons ratio for experimental data
</commit_message>
<xml_diff>
--- a/optimiser/input/__index__.xlsx
+++ b/optimiser/input/__index__.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37E612E-5759-4135-A3B1-6F95B9947D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEBC61-1C44-487D-B64C-5DBBFC95A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="225" windowWidth="28575" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="inl_1" sheetId="3" r:id="rId1"/>
-    <sheet name="inl_2" sheetId="14" r:id="rId2"/>
-    <sheet name="kaeri_1" sheetId="10" r:id="rId3"/>
-    <sheet name="kaeri_2" sheetId="11" r:id="rId4"/>
-    <sheet name="kaeri_3" sheetId="12" r:id="rId5"/>
-    <sheet name="tensile" sheetId="15" r:id="rId6"/>
+    <sheet name="notes" sheetId="16" r:id="rId1"/>
+    <sheet name="inl_1" sheetId="3" r:id="rId2"/>
+    <sheet name="inl_2" sheetId="14" r:id="rId3"/>
+    <sheet name="kaeri_1" sheetId="10" r:id="rId4"/>
+    <sheet name="kaeri_2" sheetId="11" r:id="rId5"/>
+    <sheet name="kaeri_3" sheetId="12" r:id="rId6"/>
+    <sheet name="tensile" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="273">
   <si>
     <t>temp</t>
   </si>
@@ -837,6 +838,18 @@
   </si>
   <si>
     <t>AirBase_900_25_b</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>youngs</t>
+  </si>
+  <si>
+    <t>MPa</t>
   </si>
 </sst>
 </file>
@@ -1897,6 +1910,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05C7426-797A-4E08-8D89-586E3BDD972F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72057042-979B-4A98-BA2E-14DCB6564B56}">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -2784,7 +2834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9578FDA3-F26E-4E35-80A8-9B064AEAD5AE}">
   <dimension ref="A1:M30"/>
   <sheetViews>
@@ -3854,7 +3904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539DB0F7-233D-4937-914F-C567FE238855}">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -4270,11 +4320,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69278EA8-6F9F-49D4-BBEE-C6F7D2601391}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -5909,7 +5959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F7E390-41A9-48B3-83EA-F302D713C1F5}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -6176,7 +6226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B40DCC4-4342-4D5A-B0F8-BA9AA3EEED9C}">
   <dimension ref="A1:K10"/>
   <sheetViews>

</xml_diff>